<commit_message>
updated boms with antenna
</commit_message>
<xml_diff>
--- a/sulu-ldo/sulu_ldo_bom.xlsx
+++ b/sulu-ldo/sulu_ldo_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-ldo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447B8DAE-625A-44C2-823B-93819A72A8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE66CFA-79CD-4008-820D-65537733D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="7755" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8880" yWindow="7320" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Resistors for NRF_VDDD -&gt; VDDD divider</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/tdk-corporation/MLF1005G2R2JT000/4327831</t>
-  </si>
-  <si>
-    <t>FIXED IND 2.2UH 30MA 1.3 OHM SMD</t>
-  </si>
-  <si>
     <t>C_1.1_IN1, C_1.8_IN2</t>
   </si>
   <si>
@@ -166,6 +160,36 @@
   </si>
   <si>
     <t>Coin, 24.5mm Lithium Manganese Dioxide Battery Non-Rechargeable (Primary)</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TLV70311DBVR/7776390</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 1.1V 300MA SOT23-5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LP5907MFX-1-8-NOPB/3911201</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 1.8V 250MA SOT23-5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/MLZ1005M2R2WT000/2465140</t>
+  </si>
+  <si>
+    <t>FIXED IND 2.2UH 350MA 550MOHM SM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0733910060/1465165</t>
+  </si>
+  <si>
+    <t>CONN SMA RCPT STR 50 OHM PCB</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1052,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -1168,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P3" s="1"/>
     </row>
@@ -1214,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -1223,7 +1247,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1245,13 +1269,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1276,7 +1300,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -1295,16 +1319,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -1326,16 +1350,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -1353,9 +1377,27 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="1"/>
@@ -1363,9 +1405,21 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" si="1"/>
@@ -1373,9 +1427,18 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
updated with parts that got ordered
</commit_message>
<xml_diff>
--- a/sulu-ldo/sulu_ldo_bom.xlsx
+++ b/sulu-ldo/sulu_ldo_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-ldo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE66CFA-79CD-4008-820D-65537733D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D999F51-0560-4FA8-AB29-F0C46935706A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="7320" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6825" yWindow="6555" windowWidth="21600" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -60,9 +60,6 @@
     <t>IMU ACCEL/GYRO/COMPI2C/SPI 24QFN</t>
   </si>
   <si>
-    <t>#ITEM</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -87,36 +84,15 @@
     <t>QTY/BOARD</t>
   </si>
   <si>
-    <t>Order QTY</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 6.3V 10% X7R 0402</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR60J107ME15L/6155751</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>CAP CER 100UF 6.3V X5R 0805</t>
-  </si>
-  <si>
     <t>Murata Electronics</t>
   </si>
   <si>
-    <t>GRM21BR60J107ME15L</t>
-  </si>
-  <si>
-    <t>number of boards:</t>
-  </si>
-  <si>
-    <t>Price each @ 50</t>
-  </si>
-  <si>
-    <t>price tota</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/tdk-invensense/ICM-20948/6623535</t>
   </si>
   <si>
@@ -126,18 +102,12 @@
     <t>BT1</t>
   </si>
   <si>
-    <t>Resistors for NRF_VDDD -&gt; VDDD divider</t>
-  </si>
-  <si>
     <t>C_1.1_IN1, C_1.8_IN2</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05B104KQ5NNNC/3887169</t>
   </si>
   <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
     <t>L1, L2</t>
   </si>
   <si>
@@ -147,18 +117,12 @@
     <t>CAP CER 10UF 10V X5R 0402</t>
   </si>
   <si>
-    <t>OOS :(</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BH1000G/140383</t>
   </si>
   <si>
     <t>Battery Holder (Open) Coin, 24.5mm 1 Cell PC Pin</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/toshiba-lifestyle-products/CR2477/13283172</t>
-  </si>
-  <si>
     <t>Coin, 24.5mm Lithium Manganese Dioxide Battery Non-Rechargeable (Primary)</t>
   </si>
   <si>
@@ -171,15 +135,9 @@
     <t>IC REG LINEAR 1.1V 300MA SOT23-5</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/LP5907MFX-1-8-NOPB/3911201</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
-    <t>IC REG LINEAR 1.8V 250MA SOT23-5</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/tdk-corporation/MLZ1005M2R2WT000/2465140</t>
   </si>
   <si>
@@ -190,6 +148,90 @@
   </si>
   <si>
     <t>CONN SMA RCPT STR 50 OHM PCB</t>
+  </si>
+  <si>
+    <t>RES 66.5K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Detailed description</t>
+  </si>
+  <si>
+    <t>0.1 µF ±10% 6.3V Ceramic Capacitor X7R 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>Accelerometer, Gyroscope, Magnetometer, 9 Axis Sensor I²C, SPI Output</t>
+  </si>
+  <si>
+    <t>CAP CER 100UF 2.5V X5R 0805</t>
+  </si>
+  <si>
+    <t>100 µF ±20% 2.5V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>GRM21BR60E107ME15L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR60E107ME15L/6155809</t>
+  </si>
+  <si>
+    <t>BH1000G</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jauch-quartz/CR-2477-JAUCH-(IB)/9561010</t>
+  </si>
+  <si>
+    <t>BATT LITHIUM COIN 3.0V</t>
+  </si>
+  <si>
+    <t>Shielded Multilayer Inductor 550mOhm 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>MLZ1005M2R2WT000</t>
+  </si>
+  <si>
+    <t>CR 2477 JAUCH (IB)</t>
+  </si>
+  <si>
+    <t>Linear Voltage Regulator IC Positive Fixed 1 Output 300mA SOT-23-5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/NCV8163ASN180T1G/9749431</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 1.8V 250MA 5TSOP</t>
+  </si>
+  <si>
+    <t>Linear Voltage Regulator IC Positive Fixed 1 Output 250mA 5-TSOP</t>
+  </si>
+  <si>
+    <t>SMA Connector Receptacle, Female Socket 50Ohm Through Hole Solder</t>
+  </si>
+  <si>
+    <t>RES 42.2K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>42.2 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RMCF0402FT42K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0402FT42K2/1714724</t>
+  </si>
+  <si>
+    <t>66.5 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RMCF0402FT66K5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0402FT66K5/1761639</t>
   </si>
 </sst>
 </file>
@@ -1049,21 +1091,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="3"/>
@@ -1072,57 +1113,45 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
       </c>
       <c r="O1">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1131,39 +1160,28 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>3</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J12" si="0">I2*$O$1</f>
-        <v>150</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1.44E-2</v>
-      </c>
-      <c r="L2" s="3">
-        <f t="shared" ref="L2:L12" si="1">K2*$O$1</f>
-        <v>0.72</v>
       </c>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1172,283 +1190,232 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I3">
         <v>1</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0.89739999999999998</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="1"/>
-        <v>44.87</v>
-      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="1"/>
-        <v>70.7</v>
-      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="1"/>
-        <v>37.5</v>
-      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
+      <c r="A7" t="s">
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
       </c>
       <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
+        <v>57</v>
+      </c>
+      <c r="E8">
+        <v>733910060</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" si="1"/>
-        <v>10.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0.1804</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="1"/>
-        <v>9.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L20" s="3">
-        <f>SUM(L1:L19)</f>
-        <v>173.21</v>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
put inductor on reg bom
</commit_message>
<xml_diff>
--- a/sulu-ldo/sulu_ldo_bom.xlsx
+++ b/sulu-ldo/sulu_ldo_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-ldo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D999F51-0560-4FA8-AB29-F0C46935706A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F90638-4A07-4590-92CE-6BA6232A71B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="6555" windowWidth="21600" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61455" yWindow="3855" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -108,9 +108,6 @@
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05B104KQ5NNNC/3887169</t>
   </si>
   <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05A106MP8NUB8/5961314</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/tdk-corporation/MLZ1005M2R2WT000/2465140</t>
-  </si>
-  <si>
-    <t>FIXED IND 2.2UH 350MA 550MOHM SM</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/molex/0733910060/1465165</t>
   </si>
   <si>
@@ -181,12 +172,6 @@
   </si>
   <si>
     <t>BATT LITHIUM COIN 3.0V</t>
-  </si>
-  <si>
-    <t>Shielded Multilayer Inductor 550mOhm 0402 (1005 Metric)</t>
-  </si>
-  <si>
-    <t>MLZ1005M2R2WT000</t>
   </si>
   <si>
     <t>CR 2477 JAUCH (IB)</t>
@@ -1091,9 +1076,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1116,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1148,7 +1135,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1178,7 +1165,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1205,10 +1192,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -1217,13 +1204,13 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -1231,22 +1218,22 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1254,19 +1241,19 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1274,7 +1261,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -1283,7 +1270,7 @@
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -1291,10 +1278,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>733910060</v>
@@ -1303,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1311,22 +1298,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1334,22 +1321,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1357,19 +1344,19 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1377,45 +1364,22 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I12">
         <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>